<commit_message>
Corrigindo os dados do Amazonas
</commit_message>
<xml_diff>
--- a/AM/arquivos/Análises Linchamento.xlsx
+++ b/AM/arquivos/Análises Linchamento.xlsx
@@ -792,7 +792,7 @@
     <xdr:ext cx="5448300" cy="2790825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image10.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -820,7 +820,7 @@
     <xdr:ext cx="5448300" cy="2790825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image9.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -853,7 +853,7 @@
     <xdr:ext cx="5448300" cy="2790825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -881,7 +881,7 @@
     <xdr:ext cx="5448300" cy="2790825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image7.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -994,7 +994,7 @@
     <xdr:ext cx="5448300" cy="2790825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image10.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1055,7 +1055,7 @@
     <xdr:ext cx="5448300" cy="2790825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image8.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1083,7 +1083,7 @@
     <xdr:ext cx="5448300" cy="2790825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image6.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>

</xml_diff>